<commit_message>
Working on my EDA. Interim work.
</commit_message>
<xml_diff>
--- a/CH-094 Two Column Text.xlsx
+++ b/CH-094 Two Column Text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{F9438412-9058-4BBC-9E98-D29E412CCC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23DDCAEE-CE1B-49CE-A099-C0B54B291315}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{F9438412-9058-4BBC-9E98-D29E412CCC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF05BA7A-C576-458F-90F0-1B5951ED81CD}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="23">
   <si>
     <t>Group</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7227055920810188800/</t>
+  </si>
+  <si>
+    <t>This is very clever.</t>
   </si>
 </sst>
 </file>
@@ -1679,10 +1682,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC647C1-C74A-47F5-8F41-353F47EA5968}">
-  <dimension ref="A1:P112"/>
+  <dimension ref="A1:T112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1693,9 +1696,10 @@
     <col min="7" max="7" width="15.08203125" customWidth="1"/>
     <col min="8" max="8" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="28" t="s">
         <v>18</v>
       </c>
@@ -1706,7 +1710,7 @@
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
@@ -1726,8 +1730,29 @@
       <c r="J2" s="13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="M2" s="2" t="str" cm="1">
+        <f t="array" ref="M2:N4">_xlfn.WRAPROWS(_xlfn._xlws.FILTER(C3:C13, B3:B13="b"), 2)</f>
+        <v>t4</v>
+      </c>
+      <c r="N2" s="2" t="str">
+        <v>t5</v>
+      </c>
+      <c r="P2" s="2" t="str" cm="1">
+        <f t="array" ref="P2:P4">REPT("b",_xlfn.SEQUENCE(ROWS(_xlfn.ANCHORARRAY(M2)))^0)</f>
+        <v>b</v>
+      </c>
+      <c r="R2" s="2" t="str" cm="1">
+        <f t="array" ref="R2:T2">REPT("b",{1,1,1})</f>
+        <v>b</v>
+      </c>
+      <c r="S2" s="2" t="str">
+        <v>b</v>
+      </c>
+      <c r="T2" s="2" t="str">
+        <v>b</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
@@ -1749,9 +1774,17 @@
       </c>
       <c r="K3" s="8"/>
       <c r="L3"/>
-      <c r="P3"/>
-    </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="M3" s="2" t="str">
+        <v>t6</v>
+      </c>
+      <c r="N3" s="2" t="str">
+        <v>t7</v>
+      </c>
+      <c r="P3" t="str">
+        <v>b</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
@@ -1771,9 +1804,25 @@
       <c r="J4" s="18"/>
       <c r="K4" s="8"/>
       <c r="L4"/>
-      <c r="P4"/>
-    </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="M4" s="2" t="str">
+        <v>t8</v>
+      </c>
+      <c r="N4" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P4" t="str">
+        <v>b</v>
+      </c>
+      <c r="R4" s="2" t="str" cm="1">
+        <f t="array" ref="R4:R6">REPT("b",{1;1;1})</f>
+        <v>b</v>
+      </c>
+      <c r="T4" s="2" t="str" cm="1">
+        <f t="array" ref="T4:T6">REPT("b",{1;3;1})</f>
+        <v>b</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
@@ -1796,8 +1845,14 @@
       <c r="K5" s="8"/>
       <c r="L5"/>
       <c r="P5"/>
-    </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="R5" s="2" t="str">
+        <v>b</v>
+      </c>
+      <c r="T5" s="2" t="str">
+        <v>bbb</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
@@ -1820,8 +1875,14 @@
       <c r="K6" s="8"/>
       <c r="L6"/>
       <c r="P6"/>
-    </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="R6" s="2" t="str">
+        <v>b</v>
+      </c>
+      <c r="T6" s="2" t="str">
+        <v>b</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>6</v>
       </c>
@@ -1842,7 +1903,7 @@
       <c r="L7"/>
       <c r="P7"/>
     </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
@@ -1865,8 +1926,11 @@
       <c r="K8"/>
       <c r="L8"/>
       <c r="P8"/>
-    </row>
-    <row r="9" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="Q8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
@@ -1888,7 +1952,7 @@
       <c r="L9"/>
       <c r="P9"/>
     </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
@@ -1909,7 +1973,7 @@
       <c r="O10"/>
       <c r="P10"/>
     </row>
-    <row r="11" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
         <v>11</v>
       </c>
@@ -1930,7 +1994,7 @@
       <c r="O11"/>
       <c r="P11"/>
     </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B12" s="26" t="s">
         <v>11</v>
       </c>
@@ -1951,7 +2015,7 @@
       <c r="O12"/>
       <c r="P12"/>
     </row>
-    <row r="13" spans="1:16" ht="14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="14" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
@@ -1966,7 +2030,7 @@
       <c r="I13"/>
       <c r="J13"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1976,7 +2040,7 @@
       <c r="I14"/>
       <c r="J14"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="9"/>
       <c r="D15" s="7"/>
@@ -1987,7 +2051,7 @@
       <c r="I15"/>
       <c r="J15"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="9"/>
       <c r="D16" s="7"/>
@@ -2022,7 +2086,10 @@
         <v>Column2</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B18)</f>
+        <v>=REDUCE(HSTACK(B2, "Column"&amp;{1,2}), UNIQUE(B3:B13), LAMBDA(i,x, LET(w, WRAPROWS(FILTER(C3:C13, B3:B13=x), 2), IFNA(VSTACK(i, HSTACK(REPT(x, SEQUENCE(ROWS(w))^0), w)), ""))))</v>
+      </c>
       <c r="G18" s="7"/>
       <c r="H18"/>
       <c r="I18"/>

</xml_diff>

<commit_message>
Completed review of Alt2
</commit_message>
<xml_diff>
--- a/CH-094 Two Column Text.xlsx
+++ b/CH-094 Two Column Text.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{F9438412-9058-4BBC-9E98-D29E412CCC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF05BA7A-C576-458F-90F0-1B5951ED81CD}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{F9438412-9058-4BBC-9E98-D29E412CCC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51665EF9-18FB-4323-B42C-529EFC53D4D1}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
-    <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt1" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$C$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$B$2:$C$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt2'!$B$2:$C$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$C$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="26">
   <si>
     <t>Group</t>
   </si>
@@ -132,6 +134,15 @@
   </si>
   <si>
     <t>This is very clever.</t>
+  </si>
+  <si>
+    <t>This approach is interesting because it augmented the original list with the required blanks and NAs.</t>
+  </si>
+  <si>
+    <t>An NA is required if Column 1 and Column 2 are complete an anything added needs to</t>
+  </si>
+  <si>
+    <t>be filtered out.</t>
   </si>
 </sst>
 </file>
@@ -386,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -467,6 +478,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1685,7 +1699,7 @@
   <dimension ref="A1:T112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2143,7 +2157,10 @@
         <v>t5</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="e" cm="1">
+        <f t="array" ref="F21">_xlfn.REDUCE(_xlfn.HSTACK(B2, "Column"&amp;{1,2}), _xlfn.UNIQUE(B3:B13), _xlfn.LAMBDA(_xlpm.i,_xlpm.x, _xlfn.LET(_xlpm.zz, _xlfn.UNIQUE(B3:B13),_xlpm.w, _xlfn.WRAPROWS(_xlfn._xlws.FILTER(C3:C13, B3:B13=_xlpm.x), 2), _xlfn.IFNA(_xlfn.VSTACK(_xlpm.i, _xlfn.HSTACK(_xlfn.SINGLE(+_xlpm.zz:_xlpm.x), _xlpm.w)), ""))))</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21"/>
       <c r="I21"/>
@@ -2166,6 +2183,891 @@
       <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="9" t="str">
+        <v>b</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <v>t8</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="str">
+        <v>c</v>
+      </c>
+      <c r="C24" s="4" t="str">
+        <v>t9</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <v>t10</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="str">
+        <v>d</v>
+      </c>
+      <c r="C25" s="4" t="str">
+        <v>t11</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="9"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="9"/>
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="9"/>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="9"/>
+      <c r="H42" s="9"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="9"/>
+      <c r="H43" s="9"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="9"/>
+      <c r="H44" s="9"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="9"/>
+      <c r="H45" s="9"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="9"/>
+      <c r="H46" s="9"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="9"/>
+      <c r="H47" s="9"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="9"/>
+      <c r="H48" s="9"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="9"/>
+      <c r="H49" s="9"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="H50" s="9"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="9"/>
+      <c r="H51" s="9"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="9"/>
+      <c r="H52" s="9"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="9"/>
+      <c r="H53" s="9"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="9"/>
+      <c r="H54" s="9"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="9"/>
+      <c r="H55" s="9"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="9"/>
+      <c r="H56" s="9"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="9"/>
+      <c r="H57" s="9"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="9"/>
+      <c r="H58" s="9"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="9"/>
+      <c r="H59" s="9"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="9"/>
+      <c r="H60" s="9"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="9"/>
+      <c r="H61" s="9"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="9"/>
+      <c r="H62" s="9"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="9"/>
+      <c r="H63" s="9"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="9"/>
+      <c r="H64" s="9"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="9"/>
+      <c r="H65" s="9"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="9"/>
+      <c r="H66" s="9"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="9"/>
+      <c r="H67" s="9"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="9"/>
+      <c r="H68" s="9"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="9"/>
+      <c r="H69" s="9"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="9"/>
+      <c r="H70" s="9"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="9"/>
+      <c r="H71" s="9"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="9"/>
+      <c r="H72" s="9"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="9"/>
+      <c r="H73" s="9"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="9"/>
+      <c r="H74" s="9"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="9"/>
+      <c r="H75" s="9"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="9"/>
+      <c r="H76" s="9"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="9"/>
+      <c r="H77" s="9"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="9"/>
+      <c r="H78" s="9"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="9"/>
+      <c r="H79" s="9"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="9"/>
+      <c r="H80" s="9"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="9"/>
+      <c r="H81" s="9"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H82" s="9"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H83" s="9"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H84" s="9"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H85" s="9"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H86" s="9"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H87" s="9"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H88" s="9"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H89" s="9"/>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H90" s="9"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H91" s="9"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H92" s="9"/>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H93" s="9"/>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H94" s="9"/>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H95" s="9"/>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H96" s="9"/>
+    </row>
+    <row r="97" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H97" s="9"/>
+    </row>
+    <row r="98" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H98" s="9"/>
+    </row>
+    <row r="99" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H99" s="9"/>
+    </row>
+    <row r="100" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H100" s="9"/>
+    </row>
+    <row r="101" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H101" s="9"/>
+    </row>
+    <row r="102" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H102" s="9"/>
+    </row>
+    <row r="103" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H103" s="9"/>
+    </row>
+    <row r="104" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H104" s="9"/>
+    </row>
+    <row r="105" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H105" s="9"/>
+    </row>
+    <row r="106" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H106" s="9"/>
+    </row>
+    <row r="107" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H107" s="9"/>
+    </row>
+    <row r="108" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H108" s="9"/>
+    </row>
+    <row r="109" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H109" s="9"/>
+    </row>
+    <row r="110" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H110" s="9"/>
+    </row>
+    <row r="111" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H111" s="9"/>
+    </row>
+    <row r="112" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H112" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562A3433-6502-4BB4-B104-B20B55CB1017}">
+  <dimension ref="A1:P112"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.08203125" customWidth="1"/>
+    <col min="2" max="3" width="12.58203125" style="4" customWidth="1"/>
+    <col min="4" max="6" width="12.25" customWidth="1"/>
+    <col min="7" max="7" width="15.08203125" customWidth="1"/>
+    <col min="8" max="8" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="H1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="M1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="L3"/>
+      <c r="P3"/>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="18"/>
+      <c r="K4" s="8"/>
+      <c r="L4"/>
+      <c r="P4"/>
+    </row>
+    <row r="5" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5"/>
+      <c r="P5"/>
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6"/>
+      <c r="P6"/>
+    </row>
+    <row r="7" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="18"/>
+      <c r="L7"/>
+      <c r="P7"/>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="P8"/>
+    </row>
+    <row r="9" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="P9"/>
+    </row>
+    <row r="10" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+    </row>
+    <row r="11" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B11" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+    </row>
+    <row r="12" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B12" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+    </row>
+    <row r="13" spans="1:16" ht="14" x14ac:dyDescent="0.3">
+      <c r="B13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="9"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="9"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="9"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="9"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="31" t="str" cm="1">
+        <f t="array" ref="B19:D25">_xlfn.LET(
+_xlpm.g, B3:B13,
+_xlpm.ug, _xlfn.UNIQUE(_xlpm.g),
+_xlpm.t, C3:C13,
+_xlpm.a, _xlfn.HSTACK(_xlpm.ug, IF(MOD(COUNTIFS(_xlpm.g, _xlpm.ug),2)=1,"",NA())),
+_xlpm.b, _xlfn.WRAPROWS(_xlfn.TOCOL(_xlfn.TAKE(_xlfn._xlws.SORT(_xlfn.VSTACK(_xlfn.HSTACK(_xlpm.g,_xlpm.t),_xlpm.a),1),,-1),3),2),
+_xlfn.HSTACK(_xlfn.XLOOKUP(_xlfn.TAKE(_xlpm.b,,1),_xlpm.t,_xlpm.g),_xlpm.b)
+)</f>
+        <v>a</v>
+      </c>
+      <c r="C19" s="4" t="str">
+        <v>t1</v>
+      </c>
+      <c r="D19" s="7" t="str">
+        <v>t2</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="str" cm="1">
+        <f t="array" ref="F19:G22">_xlfn.LET(
+_xlpm.g, B3:B13,
+_xlpm.ug, _xlfn.UNIQUE(_xlpm.g),
+_xlpm.t, C3:C13,
+_xlpm.a, _xlfn.HSTACK(_xlpm.ug, IF(MOD(COUNTIFS(_xlpm.g, _xlpm.ug),2)=1,"",NA())),
+_xlpm.b, _xlfn.WRAPROWS(_xlfn.TOCOL(_xlfn.TAKE(_xlfn._xlws.SORT(_xlfn.VSTACK(_xlfn.HSTACK(_xlpm.g,_xlpm.t),_xlpm.a),1),,-1),3),2),
+_xlpm.a
+)</f>
+        <v>a</v>
+      </c>
+      <c r="G19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H19"/>
+      <c r="I19" t="str" cm="1">
+        <f t="array" ref="I19:J22">_xlfn.LET(
+_xlpm.g, B3:B13,
+_xlpm.ug, _xlfn.UNIQUE(_xlpm.g),
+_xlpm.t, C3:C13,
+_xlpm.a, _xlfn.HSTACK(_xlpm.ug, IF(MOD(COUNTIFS(_xlpm.g, _xlpm.ug),2)=1,"",NA())),
+_xlpm.b, _xlfn.WRAPROWS(_xlfn.TOCOL(_xlfn.TAKE(_xlfn._xlws.SORT(_xlfn.VSTACK(_xlfn.HSTACK(_xlpm.g,_xlpm.t),_xlpm.a),1),,-1),3),2),
+_xlpm.a
+)</f>
+        <v>a</v>
+      </c>
+      <c r="J19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="9" t="str">
+        <v>a</v>
+      </c>
+      <c r="C20" s="4" t="str">
+        <v>t3</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1" t="str">
+        <v>b</v>
+      </c>
+      <c r="G20" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H20"/>
+      <c r="I20" t="str">
+        <v>b</v>
+      </c>
+      <c r="J20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="9" t="str">
+        <v>b</v>
+      </c>
+      <c r="C21" s="4" t="str">
+        <v>t4</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <v>t5</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1" t="str">
+        <v>c</v>
+      </c>
+      <c r="G21" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21" t="str">
+        <v>c</v>
+      </c>
+      <c r="J21" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="9" t="str">
+        <v>b</v>
+      </c>
+      <c r="C22" s="4" t="str">
+        <v>t6</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <v>t7</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1" t="str">
+        <v>d</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <v/>
+      </c>
+      <c r="H22"/>
+      <c r="I22" t="str">
+        <v>d</v>
+      </c>
+      <c r="J22" t="str">
+        <v/>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>

</xml_diff>

<commit_message>
Finally got an EDA that I liked
</commit_message>
<xml_diff>
--- a/CH-094 Two Column Text.xlsx
+++ b/CH-094 Two Column Text.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{F9438412-9058-4BBC-9E98-D29E412CCC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51665EF9-18FB-4323-B42C-529EFC53D4D1}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{F9438412-9058-4BBC-9E98-D29E412CCC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F0AC299-C325-45E6-838B-30ABDF232B2C}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
     <sheet name="Alt2" sheetId="3" r:id="rId3"/>
+    <sheet name="EDA" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$B$2:$C$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt2'!$B$2:$C$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">EDA!$B$2:$C$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$C$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="26">
   <si>
     <t>Group</t>
   </si>
@@ -189,7 +191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +213,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -470,6 +478,9 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -479,9 +490,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,6 +685,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -937,15 +953,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="H1" s="29" t="s">
+      <c r="C1" s="29"/>
+      <c r="H1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="M1" s="5" t="s">
         <v>21</v>
       </c>
@@ -1698,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC647C1-C74A-47F5-8F41-353F47EA5968}">
   <dimension ref="A1:T112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1714,15 +1730,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="H1" s="29" t="s">
+      <c r="C1" s="29"/>
+      <c r="H1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:20" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
@@ -2157,10 +2173,7 @@
         <v>t5</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="1" t="e" cm="1">
-        <f t="array" ref="F21">_xlfn.REDUCE(_xlfn.HSTACK(B2, "Column"&amp;{1,2}), _xlfn.UNIQUE(B3:B13), _xlfn.LAMBDA(_xlpm.i,_xlpm.x, _xlfn.LET(_xlpm.zz, _xlfn.UNIQUE(B3:B13),_xlpm.w, _xlfn.WRAPROWS(_xlfn._xlws.FILTER(C3:C13, B3:B13=_xlpm.x), 2), _xlfn.IFNA(_xlfn.VSTACK(_xlpm.i, _xlfn.HSTACK(_xlfn.SINGLE(+_xlpm.zz:_xlpm.x), _xlpm.w)), ""))))</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21"/>
       <c r="I21"/>
@@ -2608,15 +2621,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="H1" s="29" t="s">
+      <c r="C1" s="29"/>
+      <c r="H1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="M1" s="5" t="s">
         <v>21</v>
       </c>
@@ -2943,7 +2956,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="31" t="str" cm="1">
+      <c r="B19" s="28" t="str" cm="1">
         <f t="array" ref="B19:D25">_xlfn.LET(
 _xlpm.g, B3:B13,
 _xlpm.ug, _xlfn.UNIQUE(_xlpm.g),
@@ -3472,4 +3485,1122 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675AC872-3942-4B89-A6DC-DE2A460DEA10}">
+  <dimension ref="A1:V112"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.08203125" customWidth="1"/>
+    <col min="2" max="3" width="12.58203125" style="4" customWidth="1"/>
+    <col min="4" max="6" width="12.25" customWidth="1"/>
+    <col min="7" max="7" width="15.08203125" customWidth="1"/>
+    <col min="8" max="8" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="H1" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="M1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="L3"/>
+      <c r="P3"/>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="18"/>
+      <c r="K4" s="8"/>
+      <c r="L4"/>
+      <c r="P4"/>
+    </row>
+    <row r="5" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5"/>
+      <c r="P5"/>
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6"/>
+      <c r="P6"/>
+    </row>
+    <row r="7" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="18"/>
+      <c r="L7"/>
+      <c r="P7"/>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="P8"/>
+    </row>
+    <row r="9" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="P9"/>
+    </row>
+    <row r="10" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+    </row>
+    <row r="11" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B11" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+    </row>
+    <row r="12" spans="1:16" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B12" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+    </row>
+    <row r="13" spans="1:16" ht="14" x14ac:dyDescent="0.3">
+      <c r="B13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="9"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="9"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="9"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="9"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="9"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="9" t="str" cm="1">
+        <f t="array" ref="B20:B23">_xlfn.UNIQUE(B3:B13)</f>
+        <v>a</v>
+      </c>
+      <c r="C20" s="4" cm="1">
+        <f t="array" ref="C20:C23">COUNTIF(B3:B13,_xlfn.ANCHORARRAY(B20))</f>
+        <v>3</v>
+      </c>
+      <c r="D20" s="32">
+        <f>MOD(C20,2)</f>
+        <v>1</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="34" t="str" cm="1">
+        <f t="array" ref="F20:G22">_xlfn.DROP(_xlfn.REDUCE("",_xlfn.SEQUENCE(ROWS(_xlfn.ANCHORARRAY($B$20))),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(INDEX($D$20:$D$23,_xlpm.v),_xlfn.VSTACK(_xlpm.a,_xlfn.HSTACK(INDEX(_xlfn.ANCHORARRAY($B$20),_xlpm.v),"")),_xlpm.a))),1)</f>
+        <v>a</v>
+      </c>
+      <c r="G20" s="35" t="str">
+        <v/>
+      </c>
+      <c r="H20" s="33" t="str" cm="1">
+        <f t="array" ref="H20:I33">_xlfn._xlws.SORT(_xlfn.VSTACK(B3:C13,_xlfn.ANCHORARRAY(F20)))</f>
+        <v>a</v>
+      </c>
+      <c r="I20" s="33" t="str">
+        <v>t1</v>
+      </c>
+      <c r="K20" t="str" cm="1">
+        <f t="array" ref="K20:K26">_xlfn.DROP(_xlfn.XLOOKUP(_xlfn.ANCHORARRAY(M20),C3:C13,B3:B13),,-1)</f>
+        <v>a</v>
+      </c>
+      <c r="M20" t="str" cm="1">
+        <f t="array" ref="M20:N26">_xlfn.WRAPROWS(_xlfn.TAKE(_xlfn.ANCHORARRAY(H20),,-1),2)</f>
+        <v>t1</v>
+      </c>
+      <c r="N20" t="str">
+        <v>t2</v>
+      </c>
+      <c r="P20" t="str" cm="1">
+        <f t="array" ref="P20:R26">_xlfn.HSTACK(_xlfn.ANCHORARRAY(K20),_xlfn.ANCHORARRAY(M20))</f>
+        <v>a</v>
+      </c>
+      <c r="Q20" t="str">
+        <v>t1</v>
+      </c>
+      <c r="R20" t="str">
+        <v>t2</v>
+      </c>
+      <c r="T20" t="b" cm="1">
+        <f t="array" ref="T20:V26">H3:J9=_xlfn.ANCHORARRAY(P20)</f>
+        <v>1</v>
+      </c>
+      <c r="U20" t="b">
+        <v>1</v>
+      </c>
+      <c r="V20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="9" t="str">
+        <v>b</v>
+      </c>
+      <c r="C21" s="4">
+        <v>5</v>
+      </c>
+      <c r="D21" s="32">
+        <f t="shared" ref="D21:D23" si="0">MOD(C21,2)</f>
+        <v>1</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="34" t="str">
+        <v>b</v>
+      </c>
+      <c r="G21" s="35" t="str">
+        <v/>
+      </c>
+      <c r="H21" s="33" t="str">
+        <v>a</v>
+      </c>
+      <c r="I21" s="33" t="str">
+        <v>t2</v>
+      </c>
+      <c r="K21" t="str">
+        <v>a</v>
+      </c>
+      <c r="M21" t="str">
+        <v>t3</v>
+      </c>
+      <c r="N21" t="str">
+        <v/>
+      </c>
+      <c r="P21" t="str">
+        <v>a</v>
+      </c>
+      <c r="Q21" t="str">
+        <v>t3</v>
+      </c>
+      <c r="R21" t="str">
+        <v/>
+      </c>
+      <c r="T21" t="b">
+        <v>1</v>
+      </c>
+      <c r="U21" t="b">
+        <v>1</v>
+      </c>
+      <c r="V21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="9" t="str">
+        <v>c</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2</v>
+      </c>
+      <c r="D22" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="34" t="str">
+        <v>d</v>
+      </c>
+      <c r="G22" s="35" t="str">
+        <v/>
+      </c>
+      <c r="H22" s="33" t="str">
+        <v>a</v>
+      </c>
+      <c r="I22" s="33" t="str">
+        <v>t3</v>
+      </c>
+      <c r="K22" t="str">
+        <v>b</v>
+      </c>
+      <c r="M22" t="str">
+        <v>t4</v>
+      </c>
+      <c r="N22" t="str">
+        <v>t5</v>
+      </c>
+      <c r="P22" t="str">
+        <v>b</v>
+      </c>
+      <c r="Q22" t="str">
+        <v>t4</v>
+      </c>
+      <c r="R22" t="str">
+        <v>t5</v>
+      </c>
+      <c r="T22" t="b">
+        <v>1</v>
+      </c>
+      <c r="U22" t="b">
+        <v>1</v>
+      </c>
+      <c r="V22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="9" t="str">
+        <v>d</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+      <c r="D23" s="32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="H23" s="33" t="str">
+        <v>a</v>
+      </c>
+      <c r="I23" s="33" t="str">
+        <v/>
+      </c>
+      <c r="K23" t="str">
+        <v>b</v>
+      </c>
+      <c r="M23" t="str">
+        <v>t6</v>
+      </c>
+      <c r="N23" t="str">
+        <v>t7</v>
+      </c>
+      <c r="P23" t="str">
+        <v>b</v>
+      </c>
+      <c r="Q23" t="str">
+        <v>t6</v>
+      </c>
+      <c r="R23" t="str">
+        <v>t7</v>
+      </c>
+      <c r="T23" t="b">
+        <v>1</v>
+      </c>
+      <c r="U23" t="b">
+        <v>1</v>
+      </c>
+      <c r="V23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="H24" s="33" t="str">
+        <v>b</v>
+      </c>
+      <c r="I24" s="33" t="str">
+        <v>t4</v>
+      </c>
+      <c r="K24" t="str">
+        <v>b</v>
+      </c>
+      <c r="M24" t="str">
+        <v>t8</v>
+      </c>
+      <c r="N24" t="str">
+        <v/>
+      </c>
+      <c r="P24" t="str">
+        <v>b</v>
+      </c>
+      <c r="Q24" t="str">
+        <v>t8</v>
+      </c>
+      <c r="R24" t="str">
+        <v/>
+      </c>
+      <c r="T24" t="b">
+        <v>1</v>
+      </c>
+      <c r="U24" t="b">
+        <v>1</v>
+      </c>
+      <c r="V24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="H25" s="33" t="str">
+        <v>b</v>
+      </c>
+      <c r="I25" s="33" t="str">
+        <v>t5</v>
+      </c>
+      <c r="K25" t="str">
+        <v>c</v>
+      </c>
+      <c r="M25" t="str">
+        <v>t9</v>
+      </c>
+      <c r="N25" t="str">
+        <v>t10</v>
+      </c>
+      <c r="P25" t="str">
+        <v>c</v>
+      </c>
+      <c r="Q25" t="str">
+        <v>t9</v>
+      </c>
+      <c r="R25" t="str">
+        <v>t10</v>
+      </c>
+      <c r="T25" t="b">
+        <v>1</v>
+      </c>
+      <c r="U25" t="b">
+        <v>1</v>
+      </c>
+      <c r="V25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+      <c r="H26" s="33" t="str">
+        <v>b</v>
+      </c>
+      <c r="I26" s="33" t="str">
+        <v>t6</v>
+      </c>
+      <c r="K26" t="str">
+        <v>d</v>
+      </c>
+      <c r="M26" t="str">
+        <v>t11</v>
+      </c>
+      <c r="N26" t="str">
+        <v/>
+      </c>
+      <c r="P26" t="str">
+        <v>d</v>
+      </c>
+      <c r="Q26" t="str">
+        <v>t11</v>
+      </c>
+      <c r="R26" t="str">
+        <v/>
+      </c>
+      <c r="T26" t="b">
+        <v>1</v>
+      </c>
+      <c r="U26" t="b">
+        <v>1</v>
+      </c>
+      <c r="V26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="H27" s="33" t="str">
+        <v>b</v>
+      </c>
+      <c r="I27" s="33" t="str">
+        <v>t7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B28" s="9"/>
+      <c r="H28" s="33" t="str">
+        <v>b</v>
+      </c>
+      <c r="I28" s="33" t="str">
+        <v>t8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="H29" s="33" t="str">
+        <v>b</v>
+      </c>
+      <c r="I29" s="33" t="str">
+        <v/>
+      </c>
+      <c r="K29" t="str" cm="1">
+        <f t="array" ref="K29:M35">_xlfn.HSTACK(_xlfn.DROP(_xlfn.XLOOKUP(_xlfn.ANCHORARRAY(M20),C3:C13,B3:B13),,-1),_xlfn.WRAPROWS(_xlfn.TAKE(_xlfn.ANCHORARRAY(H20),,-1),2))</f>
+        <v>a</v>
+      </c>
+      <c r="L29" t="str">
+        <v>t1</v>
+      </c>
+      <c r="M29" t="str">
+        <v>t2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
+      <c r="H30" s="33" t="str">
+        <v>c</v>
+      </c>
+      <c r="I30" s="33" t="str">
+        <v>t9</v>
+      </c>
+      <c r="K30" t="str">
+        <v>a</v>
+      </c>
+      <c r="L30" t="str">
+        <v>t3</v>
+      </c>
+      <c r="M30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="H31" s="33" t="str">
+        <v>c</v>
+      </c>
+      <c r="I31" s="33" t="str">
+        <v>t10</v>
+      </c>
+      <c r="K31" t="str">
+        <v>b</v>
+      </c>
+      <c r="L31" t="str">
+        <v>t4</v>
+      </c>
+      <c r="M31" t="str">
+        <v>t5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
+      <c r="H32" s="33" t="str">
+        <v>d</v>
+      </c>
+      <c r="I32" s="33" t="str">
+        <v>t11</v>
+      </c>
+      <c r="K32" t="str">
+        <v>b</v>
+      </c>
+      <c r="L32" t="str">
+        <v>t6</v>
+      </c>
+      <c r="M32" t="str">
+        <v>t7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="H33" s="33" t="str">
+        <v>d</v>
+      </c>
+      <c r="I33" s="33" t="str">
+        <v/>
+      </c>
+      <c r="K33" t="str">
+        <v>b</v>
+      </c>
+      <c r="L33" t="str">
+        <v>t8</v>
+      </c>
+      <c r="M33" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34" t="str">
+        <v>c</v>
+      </c>
+      <c r="L34" t="str">
+        <v>t9</v>
+      </c>
+      <c r="M34" t="str">
+        <v>t10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35" t="str">
+        <v>d</v>
+      </c>
+      <c r="L35" t="str">
+        <v>t11</v>
+      </c>
+      <c r="M35" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="9"/>
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="9"/>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" s="9"/>
+      <c r="H42" s="9"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="9"/>
+      <c r="H43" s="9"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="9"/>
+      <c r="H44" s="9"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B45" s="9"/>
+      <c r="H45" s="9"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="9"/>
+      <c r="H46" s="9"/>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="9"/>
+      <c r="H47" s="9"/>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="9"/>
+      <c r="H48" s="9"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="9"/>
+      <c r="H49" s="9"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="H50" s="9"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="9"/>
+      <c r="H51" s="9"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="9"/>
+      <c r="H52" s="9"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="9"/>
+      <c r="H53" s="9"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="9"/>
+      <c r="H54" s="9"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="9"/>
+      <c r="H55" s="9"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="9"/>
+      <c r="H56" s="9"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="9"/>
+      <c r="H57" s="9"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="9"/>
+      <c r="H58" s="9"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="9"/>
+      <c r="H59" s="9"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="9"/>
+      <c r="H60" s="9"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="9"/>
+      <c r="H61" s="9"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="9"/>
+      <c r="H62" s="9"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="9"/>
+      <c r="H63" s="9"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="9"/>
+      <c r="H64" s="9"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="9"/>
+      <c r="H65" s="9"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="9"/>
+      <c r="H66" s="9"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="9"/>
+      <c r="H67" s="9"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="9"/>
+      <c r="H68" s="9"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="9"/>
+      <c r="H69" s="9"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="9"/>
+      <c r="H70" s="9"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="9"/>
+      <c r="H71" s="9"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="9"/>
+      <c r="H72" s="9"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="9"/>
+      <c r="H73" s="9"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="9"/>
+      <c r="H74" s="9"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="9"/>
+      <c r="H75" s="9"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="9"/>
+      <c r="H76" s="9"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="9"/>
+      <c r="H77" s="9"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="9"/>
+      <c r="H78" s="9"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="9"/>
+      <c r="H79" s="9"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="9"/>
+      <c r="H80" s="9"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="9"/>
+      <c r="H81" s="9"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H82" s="9"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H83" s="9"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H84" s="9"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H85" s="9"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H86" s="9"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H87" s="9"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H88" s="9"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H89" s="9"/>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H90" s="9"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H91" s="9"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H92" s="9"/>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H93" s="9"/>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H94" s="9"/>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H95" s="9"/>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H96" s="9"/>
+    </row>
+    <row r="97" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H97" s="9"/>
+    </row>
+    <row r="98" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H98" s="9"/>
+    </row>
+    <row r="99" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H99" s="9"/>
+    </row>
+    <row r="100" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H100" s="9"/>
+    </row>
+    <row r="101" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H101" s="9"/>
+    </row>
+    <row r="102" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H102" s="9"/>
+    </row>
+    <row r="103" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H103" s="9"/>
+    </row>
+    <row r="104" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H104" s="9"/>
+    </row>
+    <row r="105" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H105" s="9"/>
+    </row>
+    <row r="106" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H106" s="9"/>
+    </row>
+    <row r="107" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H107" s="9"/>
+    </row>
+    <row r="108" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H108" s="9"/>
+    </row>
+    <row r="109" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H109" s="9"/>
+    </row>
+    <row r="110" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H110" s="9"/>
+    </row>
+    <row r="111" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H111" s="9"/>
+    </row>
+    <row r="112" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H112" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fully single function solution with headers
</commit_message>
<xml_diff>
--- a/CH-094 Two Column Text.xlsx
+++ b/CH-094 Two Column Text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="8_{F9438412-9058-4BBC-9E98-D29E412CCC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC2F9FA0-3243-4E83-BEF1-2221294257BA}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{F9438412-9058-4BBC-9E98-D29E412CCC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A4E989B-66CD-483F-9536-CA2573E4E709}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4607,8 +4607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE53168-E394-4725-A73A-0DC05F09D737}">
   <dimension ref="A1:V112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5304,7 +5304,7 @@
         <v>t8</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" ht="14" x14ac:dyDescent="0.3">
       <c r="B29" s="9"/>
       <c r="H29" s="30" t="str">
         <v>b</v>
@@ -5312,18 +5312,24 @@
       <c r="I29" s="30" t="str">
         <v/>
       </c>
-      <c r="K29" t="str" cm="1">
-        <f t="array" ref="K29:M35">_xlfn.LET(_xlpm.r, _xlfn.UNIQUE(B3:B13),_xlpm.p, _xlfn.DROP(_xlfn.REDUCE("",_xlfn.SEQUENCE(ROWS(_xlpm.r)),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(INDEX(MOD(COUNTIF(B3:B13,_xlpm.r),2),_xlpm.v),_xlfn.VSTACK(_xlpm.a,_xlfn.HSTACK(INDEX(_xlpm.r,_xlpm.v),"")),_xlpm.a))),1), _xlpm.z, _xlfn._xlws.SORT(_xlfn.VSTACK(B3:C13,_xlpm.p)),_xlpm.q,_xlfn.WRAPROWS(_xlfn.TAKE(_xlpm.z,,-1),2), _xlfn.DROP(_xlfn.HSTACK(_xlfn.DROP(_xlfn.XLOOKUP(_xlpm.q,C3:C13,B3:B13),,-1),_xlfn.WRAPROWS(_xlfn.TAKE(_xlpm.z,,-1),2)),-1))</f>
-        <v>a</v>
-      </c>
-      <c r="L29" t="str">
-        <v>t1</v>
-      </c>
-      <c r="M29" t="str">
-        <v>t2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K29" s="12" t="str" cm="1">
+        <f t="array" ref="K29:M36">_xlfn.LET(_xlpm.c_1, B3:B13,_xlpm.c_2, C3:C13,
+     _xlpm.r, _xlfn.UNIQUE(_xlpm.c_1),
+     _xlpm.p, _xlfn.DROP(_xlfn.REDUCE("",_xlfn.SEQUENCE(ROWS(_xlpm.r)),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(INDEX(MOD(COUNTIF(_xlpm.c_1,_xlpm.r),2),_xlpm.v),_xlfn.VSTACK(_xlpm.a,_xlfn.HSTACK(INDEX(_xlpm.r,_xlpm.v),"")),_xlpm.a))),1),
+     _xlpm.z, _xlfn._xlws.SORT(_xlfn.VSTACK(_xlfn.HSTACK(_xlpm.c_1,_xlpm.c_2),_xlpm.p)),
+     _xlpm.q, _xlfn.WRAPROWS(_xlfn.TAKE(_xlpm.z,,-1),2),
+     _xlfn.VSTACK(H2:J2,_xlfn.DROP(_xlfn.HSTACK(_xlfn.DROP(_xlfn.XLOOKUP(_xlpm.q,_xlpm.c_2,_xlpm.c_1),,-1),_xlfn.WRAPROWS(_xlfn.TAKE(_xlpm.z,,-1),2)),-1))
+)</f>
+        <v>Group</v>
+      </c>
+      <c r="L29" s="16" t="str">
+        <v>Column 1</v>
+      </c>
+      <c r="M29" s="13" t="str">
+        <v>Column 2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="14" x14ac:dyDescent="0.3">
       <c r="B30" s="9"/>
       <c r="H30" s="30" t="str">
         <v>c</v>
@@ -5331,17 +5337,17 @@
       <c r="I30" s="30" t="str">
         <v>t9</v>
       </c>
-      <c r="K30" t="str">
+      <c r="K30" s="17" t="str">
         <v>a</v>
       </c>
-      <c r="L30" t="str">
-        <v>t3</v>
-      </c>
-      <c r="M30" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L30" s="21" t="str">
+        <v>t1</v>
+      </c>
+      <c r="M30" s="18" t="str">
+        <v>t2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="14" x14ac:dyDescent="0.3">
       <c r="B31" s="9"/>
       <c r="H31" s="30" t="str">
         <v>c</v>
@@ -5349,17 +5355,17 @@
       <c r="I31" s="30" t="str">
         <v>t10</v>
       </c>
-      <c r="K31" t="str">
-        <v>b</v>
-      </c>
-      <c r="L31" t="str">
-        <v>t4</v>
-      </c>
-      <c r="M31" t="str">
-        <v>t5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K31" s="17" t="str">
+        <v>a</v>
+      </c>
+      <c r="L31" s="21" t="str">
+        <v>t3</v>
+      </c>
+      <c r="M31" s="18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="14" x14ac:dyDescent="0.3">
       <c r="B32" s="9"/>
       <c r="H32" s="30" t="str">
         <v>d</v>
@@ -5367,17 +5373,17 @@
       <c r="I32" s="30" t="str">
         <v>t11</v>
       </c>
-      <c r="K32" t="str">
+      <c r="K32" s="17" t="str">
         <v>b</v>
       </c>
-      <c r="L32" t="str">
-        <v>t6</v>
-      </c>
-      <c r="M32" t="str">
-        <v>t7</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L32" s="21" t="str">
+        <v>t4</v>
+      </c>
+      <c r="M32" s="18" t="str">
+        <v>t5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" ht="14" x14ac:dyDescent="0.3">
       <c r="B33" s="9"/>
       <c r="H33" s="30" t="str">
         <v>d</v>
@@ -5385,51 +5391,60 @@
       <c r="I33" s="30" t="str">
         <v/>
       </c>
-      <c r="K33" t="str">
+      <c r="K33" s="17" t="str">
         <v>b</v>
       </c>
-      <c r="L33" t="str">
-        <v>t8</v>
-      </c>
-      <c r="M33" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L33" s="21" t="str">
+        <v>t6</v>
+      </c>
+      <c r="M33" s="18" t="str">
+        <v>t7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" ht="14" x14ac:dyDescent="0.3">
       <c r="B34" s="9"/>
       <c r="H34"/>
       <c r="I34"/>
       <c r="J34"/>
-      <c r="K34" t="str">
-        <v>c</v>
-      </c>
-      <c r="L34" t="str">
-        <v>t9</v>
-      </c>
-      <c r="M34" t="str">
-        <v>t10</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K34" s="17" t="str">
+        <v>b</v>
+      </c>
+      <c r="L34" s="21" t="str">
+        <v>t8</v>
+      </c>
+      <c r="M34" s="18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:13" ht="14" x14ac:dyDescent="0.3">
       <c r="B35" s="9"/>
       <c r="H35"/>
       <c r="I35"/>
       <c r="J35"/>
-      <c r="K35" t="str">
-        <v>d</v>
-      </c>
-      <c r="L35" t="str">
-        <v>t11</v>
-      </c>
-      <c r="M35" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K35" s="23" t="str">
+        <v>c</v>
+      </c>
+      <c r="L35" s="24" t="str">
+        <v>t9</v>
+      </c>
+      <c r="M35" s="25" t="str">
+        <v>t10</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" ht="14" x14ac:dyDescent="0.3">
       <c r="B36" s="9"/>
       <c r="H36"/>
       <c r="I36"/>
       <c r="J36"/>
+      <c r="K36" s="19" t="str">
+        <v>d</v>
+      </c>
+      <c r="L36" s="22" t="str">
+        <v>t11</v>
+      </c>
+      <c r="M36" s="20" t="str">
+        <v/>
+      </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>

</xml_diff>